<commit_message>
fix diff between branches
</commit_message>
<xml_diff>
--- a/DiffExcel/Test/NewFile.xlsx
+++ b/DiffExcel/Test/NewFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\ExcelBDD\DiffExcel\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C57FDF-31BE-48FC-AEB5-24A808DDACFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74DEA4E1-8E2E-48B5-978D-C5270A5F9D85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{5BF0347B-583A-4762-AF9C-435A9EE60BA2}"/>
+    <workbookView xWindow="1650" yWindow="3150" windowWidth="21600" windowHeight="11385" xr2:uid="{5BF0347B-583A-4762-AF9C-435A9EE60BA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="25">
   <si>
     <t>NewA1</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>B4</t>
+  </si>
+  <si>
+    <t>hahaha</t>
   </si>
 </sst>
 </file>
@@ -470,7 +473,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -550,6 +553,9 @@
     <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>